<commit_message>
add cpu_util and ipc results
</commit_message>
<xml_diff>
--- a/M1_data/data.xlsx
+++ b/M1_data/data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudychin/Gdrive/cmu/18-743/18-743-Power-and-Performance-optimizations-for-DNNs-on-CPU-GPU/M1_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afinci/Documents/GitHub/18-743-Power-and-Performance-optimizations-for-DNNs-on-CPU-GPU/M1_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>CPU_POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,12 @@
   <si>
     <t>stringsearch (1734Mhz)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">IPC </t>
+  </si>
+  <si>
+    <t>CPU_util</t>
   </si>
 </sst>
 </file>
@@ -89,14 +95,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -126,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -401,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
@@ -416,7 +422,7 @@
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -429,8 +435,14 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -446,8 +458,14 @@
       <c r="E3">
         <v>28.52</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3">
+        <v>1.76</v>
+      </c>
+      <c r="G3">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -463,8 +481,14 @@
       <c r="E4">
         <v>28.6110925493</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4">
+        <v>1.77</v>
+      </c>
+      <c r="G4">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -480,8 +504,14 @@
       <c r="E5">
         <v>33.1640836885</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <v>1.77</v>
+      </c>
+      <c r="G5">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -497,8 +527,14 @@
       <c r="E6">
         <v>26.972843450500001</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F6">
+        <v>1.37</v>
+      </c>
+      <c r="G6">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -514,8 +550,14 @@
       <c r="E7">
         <v>27.816295979500001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F7">
+        <v>1.38</v>
+      </c>
+      <c r="G7">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -531,8 +573,14 @@
       <c r="E8">
         <v>33.965814341300003</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F8">
+        <v>1.37</v>
+      </c>
+      <c r="G8">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -548,8 +596,14 @@
       <c r="E9">
         <v>26.535587188600001</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F9">
+        <v>0.97</v>
+      </c>
+      <c r="G9">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -565,8 +619,14 @@
       <c r="E10">
         <v>28.928309497600001</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F10">
+        <v>0.99</v>
+      </c>
+      <c r="G10">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -581,6 +641,12 @@
       </c>
       <c r="E11">
         <v>31.560027553600001</v>
+      </c>
+      <c r="F11">
+        <v>0.99</v>
+      </c>
+      <c r="G11">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dnn data to excel
</commit_message>
<xml_diff>
--- a/M1_data/data.xlsx
+++ b/M1_data/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>CPU_POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +78,58 @@
   </si>
   <si>
     <t>stringsearch (1734Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alexnet (76.8Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alexnet (537.6Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alexnet (998.4Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>googlenet (76.8Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>googlenet (537.6Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>googlenet (998.4Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resnset152 (76.8Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resnet152 (537.6Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resnet152 (998.4Mhz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPU MEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>720 MB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>820 MB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2224 MB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -416,7 +468,7 @@
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -429,8 +481,11 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -447,7 +502,7 @@
         <v>28.52</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -464,7 +519,7 @@
         <v>28.6110925493</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -481,7 +536,7 @@
         <v>33.1640836885</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -498,7 +553,7 @@
         <v>26.972843450500001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -515,7 +570,7 @@
         <v>27.816295979500001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -532,7 +587,7 @@
         <v>33.965814341300003</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -549,7 +604,7 @@
         <v>26.535587188600001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -566,7 +621,7 @@
         <v>28.928309497600001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -581,6 +636,168 @@
       </c>
       <c r="E11">
         <v>31.560027553600001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1.6493560477</v>
+      </c>
+      <c r="C13">
+        <v>0.52078262350899995</v>
+      </c>
+      <c r="D13">
+        <v>34.441567291299997</v>
+      </c>
+      <c r="E13">
+        <v>30.6971039182</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1.88985</v>
+      </c>
+      <c r="C14">
+        <v>2.14049821429</v>
+      </c>
+      <c r="D14">
+        <v>36.168750000000003</v>
+      </c>
+      <c r="E14">
+        <v>32.557142857099997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>2.0312729411800001</v>
+      </c>
+      <c r="C15">
+        <v>4.5826635294100004</v>
+      </c>
+      <c r="D15">
+        <v>38.451764705899997</v>
+      </c>
+      <c r="E15">
+        <v>35.2623529412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>1.67863615561</v>
+      </c>
+      <c r="C16">
+        <v>0.57695325269700004</v>
+      </c>
+      <c r="D16">
+        <v>37.509398496199999</v>
+      </c>
+      <c r="E16">
+        <v>33.602729650199997</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>1.85158557692</v>
+      </c>
+      <c r="C17">
+        <v>2.7311394230800001</v>
+      </c>
+      <c r="D17">
+        <v>39.699038461500002</v>
+      </c>
+      <c r="E17">
+        <v>35.922596153800001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>1.9103611111100001</v>
+      </c>
+      <c r="C18">
+        <v>6.0862236111100003</v>
+      </c>
+      <c r="D18">
+        <v>42.210416666699999</v>
+      </c>
+      <c r="E18">
+        <v>39.032638888900003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>2.2093594470000002</v>
+      </c>
+      <c r="C19">
+        <v>0.59300543120500004</v>
+      </c>
+      <c r="D19">
+        <v>40.184002633299997</v>
+      </c>
+      <c r="E19">
+        <v>36.210418038199997</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2.3617817109099999</v>
+      </c>
+      <c r="C20">
+        <v>2.6490668633199999</v>
+      </c>
+      <c r="D20">
+        <v>42.306293018700003</v>
+      </c>
+      <c r="E20">
+        <v>38.3761061947</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>2.4679863013699999</v>
+      </c>
+      <c r="C21">
+        <v>5.78504657534</v>
+      </c>
+      <c r="D21">
+        <v>45.248630136999999</v>
+      </c>
+      <c r="E21">
+        <v>41.871232876699999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added slides and data for GPU
</commit_message>
<xml_diff>
--- a/M1_data/data.xlsx
+++ b/M1_data/data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afinci/Documents/GitHub/18-743-Power-and-Performance-optimizations-for-DNNs-on-CPU-GPU/M1_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudychin/Gdrive/cmu/18-743/18-743-Power-and-Performance-optimizations-for-DNNs-on-CPU-GPU/M1_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>CPU_POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,26 +86,102 @@
   <si>
     <t>CPU_util</t>
   </si>
+  <si>
+    <t>alexnet (76.8Mhz)</t>
+  </si>
+  <si>
+    <t>720 MB</t>
+  </si>
+  <si>
+    <t>alexnet (537.6Mhz)</t>
+  </si>
+  <si>
+    <t>alexnet (998.4Mhz)</t>
+  </si>
+  <si>
+    <t>googlenet (76.8Mhz)</t>
+  </si>
+  <si>
+    <t>820 MB</t>
+  </si>
+  <si>
+    <t>googlenet (537.6Mhz)</t>
+  </si>
+  <si>
+    <t>googlenet (998.4Mhz)</t>
+  </si>
+  <si>
+    <t>resnset152 (76.8Mhz)</t>
+  </si>
+  <si>
+    <t>2224 MB</t>
+  </si>
+  <si>
+    <t>resnet152 (537.6Mhz)</t>
+  </si>
+  <si>
+    <t>resnet152 (998.4Mhz)</t>
+  </si>
+  <si>
+    <t>Memory overhead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Latency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AlexNet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoogLeNet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResNet-152</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,11 +204,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -147,7 +226,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -210,7 +289,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-TW"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -327,11 +406,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1944493024"/>
-        <c:axId val="-1938969280"/>
+        <c:axId val="-1565052816"/>
+        <c:axId val="-1564769024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1944493024"/>
+        <c:axId val="-1565052816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -371,10 +450,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1938969280"/>
+        <c:crossAx val="-1564769024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -382,7 +461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1938969280"/>
+        <c:axId val="-1564769024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -429,10 +508,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1944493024"/>
+        <c:crossAx val="-1565052816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -470,7 +549,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-TW"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -484,7 +563,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -547,7 +626,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-TW"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -759,11 +838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-1938599472"/>
-        <c:axId val="-1943191344"/>
+        <c:axId val="-1565884400"/>
+        <c:axId val="-1565882080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1938599472"/>
+        <c:axId val="-1565884400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,10 +882,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1943191344"/>
+        <c:crossAx val="-1565882080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -814,7 +893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1943191344"/>
+        <c:axId val="-1565882080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,10 +941,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1938599472"/>
+        <c:crossAx val="-1565884400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -905,7 +984,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-TW"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -935,7 +1014,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-TW"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -949,7 +1028,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1012,7 +1091,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-TW"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1224,11 +1303,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-1941623136"/>
-        <c:axId val="-1941266016"/>
+        <c:axId val="-1542480800"/>
+        <c:axId val="-1542478480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1941623136"/>
+        <c:axId val="-1542480800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,10 +1347,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1941266016"/>
+        <c:crossAx val="-1542478480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1279,7 +1358,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1941266016"/>
+        <c:axId val="-1542478480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1327,10 +1406,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1941623136"/>
+        <c:crossAx val="-1542480800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1370,7 +1449,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-TW"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1400,7 +1479,1276 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>76.8 Mhz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$A$27:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AlexNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GoogLeNet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ResNet-152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(工作表1!$G$17,工作表1!$G$18,工作表1!$G$19)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.520782624</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.576953253</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.593005431</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>537.6 Mhz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$A$27:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AlexNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GoogLeNet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ResNet-152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$G$20:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.140498214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.731139423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.649066863</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>998.4 Mhz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$A$27:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AlexNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GoogLeNet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ResNet-152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$G$23:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.582663529</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.086223611</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.785046575</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1541096912"/>
+        <c:axId val="-1541095136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1541096912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1541095136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1541095136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>Power</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
+                  <a:t>(W)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1541096912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>76.8 Mhz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$A$27:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AlexNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GoogLeNet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ResNet-152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$I$17:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>537.6 Mhz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$A$27:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AlexNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GoogLeNet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ResNet-152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$I$20:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>998.4 Mhz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$A$27:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AlexNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GoogLeNet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ResNet-152</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$I$23:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1563219872"/>
+        <c:axId val="-1564515840"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1563219872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1564515840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1564515840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>Latency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1563219872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CPU Temp</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$A$17:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>alexnet (76.8Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>googlenet (76.8Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>resnset152 (76.8Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>alexnet (537.6Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>googlenet (537.6Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>resnet152 (537.6Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>alexnet (998.4Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>googlenet (998.4Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>resnet152 (998.4Mhz)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$C$17:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>30.69710392</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.60272965</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.21041804</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.55714286</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.92259615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.37610619</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.26235294</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.03263889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41.87123288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>GPU Temp</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$A$17:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>alexnet (76.8Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>googlenet (76.8Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>resnset152 (76.8Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>alexnet (537.6Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>googlenet (537.6Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>resnet152 (537.6Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>alexnet (998.4Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>googlenet (998.4Mhz)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>resnet152 (998.4Mhz)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$D$17:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>34.44156729</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.5093985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.18400263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.16875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.69903846</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.30629302</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.45176471</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42.21041667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.24863014</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1540605488"/>
+        <c:axId val="-1561165728"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1540605488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1561165728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1561165728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1540605488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1531,6 +2879,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3012,6 +4480,1515 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3108,16 +6085,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3131,6 +6108,96 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>677333</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="圖表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="圖表 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>643466</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>93133</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>118534</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="圖表 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3402,22 +6469,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G11"/>
+  <dimension ref="A2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -3437,7 +6505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3460,7 +6528,7 @@
         <v>0.193987692308</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3483,7 +6551,7 @@
         <v>2.14577347143E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3506,7 +6574,7 @@
         <v>9.2462223944200003E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3529,7 +6597,7 @@
         <v>2.1383386581500002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3552,7 +6620,7 @@
         <v>2.16706586826E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3575,7 +6643,7 @@
         <v>3.7891421159899998E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3598,7 +6666,7 @@
         <v>2.3637010676199999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3621,7 +6689,7 @@
         <v>2.1599193252699999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3642,6 +6710,245 @@
       </c>
       <c r="G11">
         <v>1.54400708522E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.649356048</v>
+      </c>
+      <c r="C17" s="1">
+        <v>30.69710392</v>
+      </c>
+      <c r="D17" s="1">
+        <v>34.441567290000002</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
+        <v>0.52078262399999997</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.678636156</v>
+      </c>
+      <c r="C18" s="1">
+        <v>33.602729650000001</v>
+      </c>
+      <c r="D18" s="1">
+        <v>37.509398500000003</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1">
+        <v>0.576953253</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.2093594470000002</v>
+      </c>
+      <c r="C19" s="1">
+        <v>36.21041804</v>
+      </c>
+      <c r="D19" s="1">
+        <v>40.184002630000002</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1">
+        <v>0.59300543100000003</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.88985</v>
+      </c>
+      <c r="C20" s="1">
+        <v>32.557142859999999</v>
+      </c>
+      <c r="D20" s="1">
+        <v>36.168750000000003</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1">
+        <v>2.140498214</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.851585577</v>
+      </c>
+      <c r="C21" s="1">
+        <v>35.922596149999997</v>
+      </c>
+      <c r="D21" s="1">
+        <v>39.699038459999997</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1">
+        <v>2.7311394230000001</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2.3617817109999999</v>
+      </c>
+      <c r="C22" s="1">
+        <v>38.376106190000002</v>
+      </c>
+      <c r="D22" s="1">
+        <v>42.306293019999998</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1">
+        <v>2.6490668629999998</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2.0312729410000001</v>
+      </c>
+      <c r="C23" s="1">
+        <v>35.26235294</v>
+      </c>
+      <c r="D23" s="1">
+        <v>38.451764709999999</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1">
+        <v>4.5826635290000004</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.9103611110000001</v>
+      </c>
+      <c r="C24" s="1">
+        <v>39.032638890000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>42.210416670000001</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
+        <v>6.0862236110000003</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.4679863009999998</v>
+      </c>
+      <c r="C25" s="1">
+        <v>41.871232880000001</v>
+      </c>
+      <c r="D25" s="1">
+        <v>45.248630140000003</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <v>5.785046575</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>